<commit_message>
Adicionando EPL 17_18 18_19
</commit_message>
<xml_diff>
--- a/de_para_siglas_epl.xlsx
+++ b/de_para_siglas_epl.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="96">
   <si>
     <t xml:space="preserve">time</t>
   </si>
@@ -302,6 +302,15 @@
   </si>
   <si>
     <t xml:space="preserve">Swansea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stoke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">West Brom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hull</t>
   </si>
 </sst>
 </file>
@@ -377,7 +386,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -392,6 +401,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -415,10 +428,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B54"/>
+  <dimension ref="A1:B57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A30" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A46" activeCellId="0" sqref="A46"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B56" activeCellId="0" sqref="A56:B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -844,8 +857,36 @@
         <v>58</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="3"/>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B57" s="4"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:B39"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>